<commit_message>
código de previsão dos ultimos 30 dias da base
</commit_message>
<xml_diff>
--- a/Codigo/resultados_previsoes.xlsx
+++ b/Codigo/resultados_previsoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arq. Andrea\Documents\Yuri\git\previsao-ibovespa\Codigo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://corptb-my.sharepoint.com/personal/yupopic_tbdir_net/Documents/000 - Pessoal/070 - VSCODE/072 - Tech Challenge/Fase 2/previsao-ibovespa/Codigo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B905631F-7CDA-41DA-88C9-C6877B538501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B905631F-7CDA-41DA-88C9-C6877B538501}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB8B4008-43CA-448E-9F12-75C0C57761E1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,21 +427,21 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +464,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45856</v>
       </c>
@@ -487,7 +487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45856</v>
       </c>
@@ -510,7 +510,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45856</v>
       </c>
@@ -533,7 +533,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45856</v>
       </c>
@@ -556,7 +556,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45856</v>
       </c>
@@ -579,7 +579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45856</v>
       </c>
@@ -602,7 +602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45856</v>
       </c>
@@ -625,7 +625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45856</v>
       </c>
@@ -648,7 +648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45856</v>
       </c>
@@ -671,7 +671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45856</v>
       </c>
@@ -694,7 +694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45856</v>
       </c>
@@ -717,7 +717,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>45856</v>
       </c>
@@ -740,7 +740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>45856</v>
       </c>
@@ -763,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>45856</v>
       </c>
@@ -786,7 +786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45856</v>
       </c>
@@ -809,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45856</v>
       </c>
@@ -832,7 +832,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45856</v>
       </c>
@@ -855,7 +855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45856</v>
       </c>
@@ -878,7 +878,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45856</v>
       </c>
@@ -901,7 +901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45856</v>
       </c>
@@ -924,7 +924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45856</v>
       </c>
@@ -947,7 +947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45856</v>
       </c>
@@ -970,7 +970,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45856</v>
       </c>
@@ -993,7 +993,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45856</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45856</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45856</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45856</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45856</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45856</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45856</v>
       </c>
@@ -1157,4 +1157,10 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{b97ea58d-47e6-47cc-9ab7-39ab03def869}" enabled="1" method="Standard" siteId="{505cca53-5750-4134-9501-8d52d5df3cd1}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>